<commit_message>
[nb] Edit: MocksY12/Group6/MockExams Group 6
</commit_message>
<xml_diff>
--- a/12BGrades.xlsx
+++ b/12BGrades.xlsx
@@ -220,7 +220,7 @@
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="1" ySplit="0" topLeftCell="S1" activePane="topRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="Z14" activeCellId="0" sqref="Z14"/>
+      <selection pane="topRight" activeCell="Z10" activeCellId="0" sqref="Z10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.40625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -784,6 +784,9 @@
       </c>
       <c r="W10" s="1" t="n">
         <v>3</v>
+      </c>
+      <c r="Z10" s="1" t="n">
+        <v>2</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>